<commit_message>
modified:   cadastro_OrdemTurmas.xlsx 	modified:   cadastro_alunos.xlsx 	modified:   cadastro_turmas.xlsx 	modified:   main.py 	modified:   mofome.kv
</commit_message>
<xml_diff>
--- a/cadastro_OrdemTurmas.xlsx
+++ b/cadastro_OrdemTurmas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,38 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1BADM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new file:   "M\303\263Fome.png" modified:   cadastro_OrdemTurmas.xlsx 	new file:   cadastro_monitores.xlsx 	modified:   cadastro_turmas.xlsx 	new file:   escolhas_turmas.xlsx 	modified:   main.py 	modified:   mofome.kv
</commit_message>
<xml_diff>
--- a/cadastro_OrdemTurmas.xlsx
+++ b/cadastro_OrdemTurmas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,64 +456,64 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1ADS</t>
+          <t>2BDS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1ADS</t>
+          <t>3AADM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -525,25 +525,121 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3ADS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2ADS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1ADS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>1</t>
         </is>

</xml_diff>

<commit_message>
mudanca de str->int na ordem_fila e salvar frequencia
</commit_message>
<xml_diff>
--- a/cadastro_OrdemTurmas.xlsx
+++ b/cadastro_OrdemTurmas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,288 +456,73 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3BDS</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+          <t>3ADS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2AADM</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+          <t>2BDS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2BDS</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+          <t>1ADS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3AADM</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1BADM</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>3ADS</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2ADS</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1ADS</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
           <t>Turma</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Segunda</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Terça</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Quarta</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Quinta</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Sexta</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mudanças na amostragem de dados cadastrados
</commit_message>
<xml_diff>
--- a/cadastro_OrdemTurmas.xlsx
+++ b/cadastro_OrdemTurmas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,23 +466,23 @@
         <v>2</v>
       </c>
       <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1ADS</t>
+          <t>3ADS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -491,14 +491,36 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
         <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
+        <is>
+          <t>2BADM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Turma</t>
         </is>

</xml_diff>